<commit_message>
export figures for costs & balance
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="report_types" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="405">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -1086,9 +1086,6 @@
     <t xml:space="preserve">PAYPAL PTE LTD | 10918001-00000001-</t>
   </si>
   <si>
-    <t xml:space="preserve">Pending</t>
-  </si>
-  <si>
     <t xml:space="preserve">NA | NA | 4476 XXXX XXXX 1025 / null</t>
   </si>
   <si>
@@ -1203,7 +1200,7 @@
     <t xml:space="preserve">ASSETS</t>
   </si>
   <si>
-    <t xml:space="preserve">Current assets</t>
+    <t xml:space="preserve">Current Assets</t>
   </si>
   <si>
     <t xml:space="preserve">Cash</t>
@@ -1227,10 +1224,10 @@
     <t xml:space="preserve">LIABILITIES</t>
   </si>
   <si>
-    <t xml:space="preserve">Current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long term</t>
+    <t xml:space="preserve">Current Liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long Term Liabilities</t>
   </si>
   <si>
     <t xml:space="preserve">Month</t>
@@ -1255,7 +1252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1289,11 +1286,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1338,7 +1330,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1372,10 +1364,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2591,8 +2579,8 @@
   </sheetPr>
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3392,8 +3380,8 @@
   </sheetPr>
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A138" activeCellId="0" sqref="A138"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4806,11 +4794,11 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="4" t="s">
+      <c r="A170" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B170" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4818,7 +4806,7 @@
         <v>154</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4826,7 +4814,7 @@
         <v>165</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4834,7 +4822,7 @@
         <v>154</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4842,10 +4830,10 @@
         <v>120</v>
       </c>
       <c r="B174" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C174" s="4" t="s">
         <v>357</v>
-      </c>
-      <c r="C174" s="4" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4853,7 +4841,7 @@
         <v>200</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4861,7 +4849,7 @@
         <v>148</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4869,7 +4857,7 @@
         <v>108</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4877,7 +4865,7 @@
         <v>144</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4885,7 +4873,7 @@
         <v>149</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4893,7 +4881,7 @@
         <v>124</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4901,15 +4889,15 @@
         <v>123</v>
       </c>
       <c r="B181" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B182" s="4" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B182" s="4" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4917,31 +4905,31 @@
         <v>112</v>
       </c>
       <c r="B183" s="4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B184" s="4" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B184" s="4" t="s">
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B185" s="4" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="9" t="s">
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B186" s="4" t="s">
         <v>369</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4949,15 +4937,15 @@
         <v>102</v>
       </c>
       <c r="B187" s="4" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B188" s="4" t="s">
         <v>371</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B188" s="4" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4965,10 +4953,10 @@
         <v>200</v>
       </c>
       <c r="B189" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C189" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="C189" s="4" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4976,7 +4964,7 @@
         <v>155</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4984,63 +4972,63 @@
         <v>154</v>
       </c>
       <c r="B191" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B192" s="4" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="9" t="s">
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B193" s="7" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B192" s="4" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B193" s="7" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="9" t="s">
+      <c r="B195" s="4" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B194" s="4" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B195" s="4" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="9" t="s">
+      <c r="B197" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B196" s="4" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B197" s="4" t="s">
+      <c r="B198" s="4" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B198" s="4" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5048,15 +5036,15 @@
         <v>112</v>
       </c>
       <c r="B199" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B200" s="4" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B200" s="4" t="s">
-        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -5077,29 +5065,29 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="10" width="17.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.74"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -5113,11 +5101,11 @@
       <c r="F1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>389</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>5</v>
@@ -5125,13 +5113,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>392</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>19310</v>
@@ -5148,10 +5136,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -5171,10 +5159,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>53</v>
@@ -5188,16 +5176,16 @@
       <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>393</v>
+      <c r="G4" s="9" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>55</v>
@@ -5211,16 +5199,16 @@
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>393</v>
+      <c r="G5" s="9" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>157</v>
@@ -5234,16 +5222,16 @@
       <c r="F6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>394</v>
+      <c r="G6" s="9" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>10</v>
@@ -5257,16 +5245,16 @@
       <c r="F7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>395</v>
+      <c r="G7" s="9" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>12</v>
@@ -5280,16 +5268,16 @@
       <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>396</v>
+      <c r="G8" s="9" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>19</v>
@@ -5309,10 +5297,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>15</v>
@@ -5332,10 +5320,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>24</v>
@@ -5355,10 +5343,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>26</v>
@@ -5378,10 +5366,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>144</v>
@@ -5398,10 +5386,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>145</v>
@@ -5418,10 +5406,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>142</v>
@@ -5438,10 +5426,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>398</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>399</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>22</v>
@@ -5464,10 +5452,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>398</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>399</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>28</v>
@@ -5490,10 +5478,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>398</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>399</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>150</v>
@@ -5510,10 +5498,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>149</v>
@@ -5530,10 +5518,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>148</v>
@@ -5566,7 +5554,7 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -5586,50 +5574,50 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>404</v>
-      </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>392</v>
-      </c>
-      <c r="B2" s="12" t="n">
+    <row r="2" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="B2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="7" t="n">
         <v>71936.2</v>
       </c>
     </row>
-    <row r="3" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+    <row r="3" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="12" t="n">
+      <c r="B3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="n">
+      <c r="D3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="7" t="n">
@@ -6125,7 +6113,7 @@
         <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>

</xml_diff>